<commit_message>
Add household data pipeline and tax burden calculation outputs
</commit_message>
<xml_diff>
--- a/Cleaning/Energy Price/energy_price_cleaned.xlsx
+++ b/Cleaning/Energy Price/energy_price_cleaned.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10204"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/zctpj17_ucl_ac_uk/Documents/ECON0053 Economics of Tax Policy/Grp Project/Quantitative/Cleaning/Energy Price/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_B61C049661172AD6A7FD9890E2AC9AB43B198F58" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA3BD8A7-6BB8-E045-B5C0-DCB0DBC29034}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_B61C049661172AD6A7FD9890E2AC9AB43B198F58" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A466CD8-F4FC-0441-B6E6-980EDCAE59FA}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="800" windowWidth="34760" windowHeight="21280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,6 +130,23 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -158,23 +175,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -188,15 +188,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B986A99A-D5DB-CB44-814C-3F315D03DB0E}" name="Table1" displayName="Table1" ref="A1:E658" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B986A99A-D5DB-CB44-814C-3F315D03DB0E}" name="Table1" displayName="Table1" ref="A1:E658" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:E658" xr:uid="{B986A99A-D5DB-CB44-814C-3F315D03DB0E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{31034DB8-8A1A-BA4D-9A2C-F39C116A88AF}" name="REF_DATE" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{31034DB8-8A1A-BA4D-9A2C-F39C116A88AF}" name="REF_DATE" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{3724C85B-26FB-F54E-954A-35E9FBCAFB02}" name="Region"/>
     <tableColumn id="3" xr3:uid="{99277602-8EFC-4542-9C69-86FBCEB03274}" name="Type of fuel"/>
     <tableColumn id="4" xr3:uid="{42C87114-9BC1-AB45-A72B-9146F2972E89}" name="UOM"/>
@@ -496,7 +492,7 @@
   <dimension ref="A1:E658"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection sqref="A1:E658"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -504,6 +500,7 @@
     <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>